<commit_message>
Add a execute,zero and op_code_functions excel file
</commit_message>
<xml_diff>
--- a/A4_pipelined_processor/op_code and functions.xlsx
+++ b/A4_pipelined_processor/op_code and functions.xlsx
@@ -1,25 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Mcgill\2017 Winter\ECSE 425\Project\ECSE425_Project\A4_pipelined_processor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mambo/Documents/University/Classes/Github/ECSE425_Project/A4_pipelined_processor/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="6970"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24640" windowHeight="13940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Fucntions for ALU" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$H$1:$H$28</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="84">
   <si>
     <t>I-type</t>
   </si>
@@ -246,12 +253,45 @@
   </si>
   <si>
     <t>ALU op_code = op_code or funct (due to no overlapping)</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t>Arithmetic</t>
+  </si>
+  <si>
+    <t>Logical</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Control Flow</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t>J-Type</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Implemented?</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -269,7 +309,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -279,44 +319,79 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -324,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -346,11 +421,82 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -662,24 +808,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="8.7265625" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="5.08984375" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="8.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="11" t="s">
@@ -704,7 +850,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -729,7 +875,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -750,7 +896,7 @@
       </c>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -771,7 +917,7 @@
       </c>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>15</v>
@@ -792,7 +938,7 @@
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>16</v>
@@ -813,7 +959,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>19</v>
@@ -834,7 +980,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>22</v>
@@ -853,7 +999,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>24</v>
@@ -872,7 +1018,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>25</v>
@@ -895,7 +1041,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
         <v>26</v>
@@ -918,7 +1064,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -945,7 +1091,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>4</v>
@@ -970,7 +1116,7 @@
       </c>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>6</v>
@@ -995,7 +1141,7 @@
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>7</v>
@@ -1020,7 +1166,7 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
@@ -1045,7 +1191,7 @@
       </c>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>10</v>
@@ -1070,7 +1216,7 @@
       </c>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
         <v>11</v>
@@ -1095,7 +1241,7 @@
       </c>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
         <v>12</v>
@@ -1120,7 +1266,7 @@
       </c>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>13</v>
@@ -1145,7 +1291,7 @@
       </c>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>17</v>
@@ -1172,7 +1318,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
         <v>18</v>
@@ -1199,7 +1345,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
         <v>20</v>
@@ -1224,7 +1370,7 @@
       </c>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
         <v>21</v>
@@ -1249,7 +1395,7 @@
       </c>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
         <v>23</v>
@@ -1274,7 +1420,7 @@
       </c>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10" t="s">
         <v>28</v>
@@ -1297,7 +1443,7 @@
       <c r="H26" s="12"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>2</v>
       </c>
@@ -1318,7 +1464,7 @@
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
         <v>29</v>
@@ -1346,4 +1492,597 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="6" max="6" width="43.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="9">
+        <v>100000</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="9">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="14"/>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="6">
+        <v>100010</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="6">
+        <v>100010</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="14"/>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="14"/>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="14"/>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="14"/>
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="14"/>
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="14"/>
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="14"/>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="14"/>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="14"/>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="14"/>
+      <c r="B13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="14"/>
+      <c r="B14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="14"/>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="14"/>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="14"/>
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="14"/>
+      <c r="B21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="A16:A22"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H2:H23">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",H2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",H2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to op_code sheet
</commit_message>
<xml_diff>
--- a/A4_pipelined_processor/op_code and functions.xlsx
+++ b/A4_pipelined_processor/op_code and functions.xlsx
@@ -421,21 +421,21 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -443,46 +443,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1499,7 +1459,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1530,12 +1490,12 @@
       <c r="G1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1556,12 +1516,12 @@
       <c r="G2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1580,12 +1540,12 @@
       <c r="G3" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1604,12 +1564,12 @@
       <c r="G4" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>83</v>
+      <c r="H4" s="16" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1628,12 +1588,12 @@
       <c r="G5" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H5" s="18" t="s">
-        <v>83</v>
+      <c r="H5" s="16" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1652,12 +1612,12 @@
       <c r="G6" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H6" s="18" t="s">
-        <v>83</v>
+      <c r="H6" s="16" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1676,12 +1636,12 @@
       <c r="G7" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
@@ -1700,12 +1660,12 @@
       <c r="G8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
@@ -1724,12 +1684,12 @@
       <c r="G9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1754,7 +1714,7 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
@@ -1779,7 +1739,7 @@
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
@@ -1804,7 +1764,7 @@
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
@@ -1824,12 +1784,12 @@
         <v>79</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1849,12 +1809,12 @@
         <v>79</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1879,7 +1839,7 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1899,12 +1859,12 @@
         <v>75</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1922,12 +1882,12 @@
         <v>75</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="4" t="s">
         <v>14</v>
       </c>
@@ -1945,12 +1905,12 @@
         <v>76</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="4" t="s">
         <v>15</v>
       </c>
@@ -1968,12 +1928,12 @@
         <v>76</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
@@ -1991,12 +1951,12 @@
         <v>76</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="4" t="s">
         <v>25</v>
       </c>
@@ -2019,7 +1979,7 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="10" t="s">
         <v>26</v>
       </c>
@@ -2042,7 +2002,7 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="14" t="s">
         <v>80</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2058,7 +2018,7 @@
       <c r="F23" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="13" t="s">
         <v>78</v>
       </c>
       <c r="H23" s="6" t="s">
@@ -2076,10 +2036,10 @@
     <mergeCell ref="A16:A22"/>
   </mergeCells>
   <conditionalFormatting sqref="H2:H23">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",H2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>